<commit_message>
correcting some pinout and drive strength issues
</commit_message>
<xml_diff>
--- a/docs/Horizon_Condor_מעקב.xlsx
+++ b/docs/Horizon_Condor_מעקב.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Horizon\Condor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEA4148-DBFE-4177-AE2D-9B9B810443EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEC6545-6B6B-4B99-A7CF-DD694AD592AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43470" yWindow="4430" windowWidth="28800" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>תאריך</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>מייל סיכום פגישה מיובל מנהל הפיתוח באלביט</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ווצאפ לבר שאי אפשר לעמוד באבן דרך לעוד יומיים כי אנחנו מחכים לתשובות </t>
+  </si>
+  <si>
+    <t>בר קיבלה את ההודעה אישרה בווצאפ</t>
   </si>
 </sst>
 </file>
@@ -453,7 +459,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -557,8 +563,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="6"/>
     </row>

</xml_diff>